<commit_message>
Found some nasty design flaws. Everything is explained in a comment near collision_handler process in HI_Datapath_Control_Unit.vhd. I already have a fix for this, but it is not implemented yet.
</commit_message>
<xml_diff>
--- a/collisions_table.xlsx
+++ b/collisions_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\unlimitedrepositoryworks_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A0C2C76-8182-4860-8DB9-FE0232F8B8ED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC3673-3928-4CCA-BFF4-1383122F4482}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1A4CB678-C40F-48FF-B024-9AD779A5851D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Alien</t>
   </si>
@@ -63,25 +63,19 @@
     <t>_ / Hide</t>
   </si>
   <si>
-    <t>Destroy / _</t>
-  </si>
-  <si>
     <t>_ / Destroy</t>
   </si>
   <si>
     <t>_ / Change Dir</t>
   </si>
   <si>
-    <t>??? / ???</t>
-  </si>
-  <si>
-    <t>???  / ???</t>
-  </si>
-  <si>
-    <t>_ / Gameover</t>
-  </si>
-  <si>
     <t>_ / _</t>
+  </si>
+  <si>
+    <t>Gameover</t>
+  </si>
+  <si>
+    <t>Hide / _</t>
   </si>
 </sst>
 </file>
@@ -106,12 +100,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -125,6 +113,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,19 +158,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -496,7 +490,7 @@
   <dimension ref="F5:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,21 +530,21 @@
     <row r="6" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>0</v>
@@ -569,7 +563,7 @@
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="6" t="s">
@@ -578,16 +572,12 @@
     </row>
     <row r="8" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H8" s="5"/>
-      <c r="I8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="4" t="s">
-        <v>18</v>
+      <c r="M8" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>1</v>
@@ -601,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -610,12 +600,10 @@
       </c>
     </row>
     <row r="10" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="N10" s="6" t="s">

</xml_diff>

<commit_message>
Added a more useful table in collision_table.xlsx, started working on destructions implementation.
</commit_message>
<xml_diff>
--- a/collisions_table.xlsx
+++ b/collisions_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\unlimitedrepositoryworks_master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EC3673-3928-4CCA-BFF4-1383122F4482}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD947D2-06A1-4B43-8B5B-A0210EE531D3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1A4CB678-C40F-48FF-B024-9AD779A5851D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Alien</t>
   </si>
@@ -76,13 +76,114 @@
   </si>
   <si>
     <t>Hide / _</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Destroy / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HP - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Destroy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / HP - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Destroy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / _</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Destroy / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Destroy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Destroy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ _</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +191,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +228,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,6 +286,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -487,20 +605,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D66C9C8-45E0-4119-BCD7-9DD8B4094ED8}">
-  <dimension ref="F5:N13"/>
+  <dimension ref="F5:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="9.140625" style="1"/>
     <col min="6" max="14" width="16.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="16" width="9.140625" style="1"/>
+    <col min="17" max="20" width="16.7109375" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
@@ -526,8 +646,18 @@
         <v>5</v>
       </c>
       <c r="N5" s="4"/>
+      <c r="Q5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
         <v>15</v>
@@ -549,8 +679,16 @@
       <c r="N6" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
@@ -569,8 +707,16 @@
       <c r="N7" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -582,8 +728,18 @@
       <c r="N8" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="Q8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I9" s="4" t="s">
         <v>10</v>
       </c>
@@ -598,8 +754,14 @@
       <c r="N9" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="10" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -609,25 +771,63 @@
       <c r="N10" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="Q11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="6:14" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:20" s="2" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M13" s="5"/>
       <c r="N13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>